<commit_message>
Hoja libro excel Practica
</commit_message>
<xml_diff>
--- a/SIPA/controlador/Reportes.xlsx
+++ b/SIPA/controlador/Reportes.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
     <sheet name="convenio" sheetId="2" r:id="rId5"/>
+    <sheet name="practica" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -33,7 +34,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -43,6 +44,9 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -51,7 +55,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -402,4 +406,32 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>